<commit_message>
Updated camera and movement
</commit_message>
<xml_diff>
--- a/Devlog.xlsx
+++ b/Devlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity Projects\Fishing-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7397AA-64AF-4D66-B3BD-5F22414D47CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2747D20-94C8-4E7F-B70D-59332AA8E70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{865F7428-D6C5-4175-847E-73F6665699E5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Issue</t>
   </si>
@@ -79,13 +79,25 @@
   </si>
   <si>
     <t>Not Started</t>
+  </si>
+  <si>
+    <t>Character animation - bare bones run anim</t>
+  </si>
+  <si>
+    <t>Inventory system</t>
+  </si>
+  <si>
+    <t>Player gear system</t>
+  </si>
+  <si>
+    <t>Fishing system - written in outline</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,11 +133,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="Proxima Nova Lt"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
       <name val="Proxima Nova Lt"/>
     </font>
     <font>
@@ -314,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -326,31 +333,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -367,6 +360,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -684,17 +691,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A0E407-8454-4A8B-B9BC-33DFC92E725B}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="73.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11" style="6" customWidth="1"/>
+    <col min="3" max="3" width="11" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
     <col min="5" max="5" width="18" style="3" customWidth="1"/>
     <col min="7" max="7" width="15.140625" style="1" customWidth="1"/>
@@ -702,29 +709,29 @@
     <col min="10" max="10" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="18" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:10" s="12" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="9"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -734,7 +741,7 @@
         <f>DATE(2021,8,18)</f>
         <v>44426</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>0.75</v>
       </c>
       <c r="D2" s="4"/>
@@ -742,14 +749,14 @@
         <f>DATE(2021,8,18)</f>
         <v>44426</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="19">
         <f>SUM(C:C)</f>
-        <v>3.55</v>
-      </c>
-      <c r="I2" s="10" t="s">
+        <v>5.05</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="11"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -759,7 +766,7 @@
         <f>DATE(2021,8,18)</f>
         <v>44426</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>0.25</v>
       </c>
       <c r="D3" s="4"/>
@@ -767,11 +774,11 @@
         <f>DATE(2021,8,18)</f>
         <v>44426</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="I3" s="10" t="s">
+      <c r="G3" s="20"/>
+      <c r="I3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="12"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -781,7 +788,7 @@
         <f>DATE(2021,8,18)</f>
         <v>44426</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>0.3</v>
       </c>
       <c r="D4" s="4"/>
@@ -789,10 +796,10 @@
         <f>DATE(2021,8,18)</f>
         <v>44426</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="14"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -802,10 +809,15 @@
         <f>DATE(2021,8,18)</f>
         <v>44426</v>
       </c>
-      <c r="C5" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D5" s="5"/>
+      <c r="C5" s="5">
+        <f>0.5+1</f>
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E6" si="0">DATE(2021,8,18)</f>
+        <v>44426</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -815,11 +827,39 @@
         <f>DATE(2021,8,18)</f>
         <v>44426</v>
       </c>
-      <c r="C6" s="6">
-        <f>0.25+1.5</f>
-        <v>1.75</v>
-      </c>
-      <c r="D6" s="7"/>
+      <c r="C6" s="5">
+        <f>0.25+1.5+0.5</f>
+        <v>2.25</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>44426</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="23"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="23"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>